<commit_message>
loop to read words
</commit_message>
<xml_diff>
--- a/Book.xlsx
+++ b/Book.xlsx
@@ -24,15 +24,57 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>1st word</t>
-  </si>
-  <si>
-    <t>2nd</t>
-  </si>
-  <si>
-    <t>3rd</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="17">
+  <si>
+    <t>sample 1</t>
+  </si>
+  <si>
+    <t>sample 2</t>
+  </si>
+  <si>
+    <t>sample 3</t>
+  </si>
+  <si>
+    <t>sample 6</t>
+  </si>
+  <si>
+    <t>sample 5</t>
+  </si>
+  <si>
+    <t>sample 4</t>
+  </si>
+  <si>
+    <t>15/04/2021</t>
+  </si>
+  <si>
+    <t>sample 7</t>
+  </si>
+  <si>
+    <t>sample 8</t>
+  </si>
+  <si>
+    <t>sample 9</t>
+  </si>
+  <si>
+    <t>sample 10</t>
+  </si>
+  <si>
+    <t>sample 11</t>
+  </si>
+  <si>
+    <t>sample 12</t>
+  </si>
+  <si>
+    <t>sample 13</t>
+  </si>
+  <si>
+    <t>sample 14</t>
+  </si>
+  <si>
+    <t>sample 15</t>
+  </si>
+  <si>
+    <t>sample 16</t>
   </si>
 </sst>
 </file>
@@ -68,8 +110,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -350,27 +393,147 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A3"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
+      </c>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>